<commit_message>
Updated files excluding plotnormfiring, copyPaste, and print.
</commit_message>
<xml_diff>
--- a/CeA CRF NPP EPHYS PAPER/DATA FILES/DATA FILES/DATA Unit Details By Hour_05072018_15h26m.xlsx
+++ b/CeA CRF NPP EPHYS PAPER/DATA FILES/DATA FILES/DATA Unit Details By Hour_05072018_15h26m.xlsx
@@ -1,48 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Dropbox (Sparta Lab)\@now\Update CRF Ephys\DATA FILES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\James\Dropbox (Personal)\Public\Science Data\Sparta Lab\Sparta-Lab-CRF-Ephys-Paper-Scripts-and-Data\CeA CRF NPP EPHYS PAPER\DATA FILES\DATA FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880BE4A1-E971-4BE9-99F3-D199BA93ED08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F1B32D-E922-4FA9-873C-C42084883836}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14028" windowHeight="9012" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="FIG2_ShortUnitDetails" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="DRINK DAYS" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Slicer_Early_Vs_Late">#N/A</definedName>
     <definedName name="Slicer_Lick_Response">#N/A</definedName>
     <definedName name="Slicer_Light_Response">#N/A</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{46BE6895-7355-4a93-B00E-2C351335B9C9}">
       <x15:slicerCaches xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicerCache r:id="rId4"/>
         <x14:slicerCache r:id="rId5"/>
         <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
       </x15:slicerCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="126">
   <si>
     <t>File Name</t>
   </si>
@@ -409,6 +416,18 @@
   <si>
     <t>Burst Duration(ms)</t>
   </si>
+  <si>
+    <t>Original Filename</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>drinkType</t>
+  </si>
+  <si>
+    <t>drinkDay</t>
+  </si>
 </sst>
 </file>
 
@@ -474,7 +493,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -497,30 +516,247 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -547,19 +783,19 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>1596736</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>954479</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>96983</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>1176251</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>294508</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>38794</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Light Response">
@@ -582,7 +818,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -625,19 +861,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>1412471</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>530728</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>1431174</xdr:colOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>157545</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Lick Response">
@@ -660,7 +896,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -703,19 +939,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1608909</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>601980</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>3443151</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>68581</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="Early Vs Late">
@@ -738,7 +974,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -822,18 +1058,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A9:AO158" totalsRowShown="0">
-  <autoFilter ref="A9:AO158" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="NR"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="8">
-      <filters>
-        <filter val="NR"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A9:AO158" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="File Name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="DATA(Q)"/>
@@ -841,14 +1066,14 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Unit Name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Drink Type"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Ethanol Day"/>
-    <tableColumn id="40" xr3:uid="{AEB23D3C-DAFE-477C-8D6D-E35EEBAE3CC2}" name="Early Vs Late" dataDxfId="1">
+    <tableColumn id="40" xr3:uid="{AEB23D3C-DAFE-477C-8D6D-E35EEBAE3CC2}" name="Early Vs Late" dataDxfId="10">
       <calculatedColumnFormula>IF(Table1[[#This Row],[Ethanol Day]]&lt;9,"Early",IF(Table1[[#This Row],[Ethanol Day]]&gt;16,"Late","Mid"))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Light Response"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Lick Response"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="#Licks"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="FullSess-Spk/sec"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Change In Rate" dataDxfId="2">
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="Change In Rate" dataDxfId="9">
       <calculatedColumnFormula>Table1[[#This Row],[Hour4-Spk/sec]]-Table1[[#This Row],[Hour1-Spk/sec]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="FullSess-%SpikesInBursts"/>
@@ -873,7 +1098,7 @@
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Avg percSpikesInBursts"/>
     <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Avg SpikesInBurst"/>
     <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="Avg MeanISIinBurst"/>
-    <tableColumn id="41" xr3:uid="{C175C68A-FBEC-43F7-9A02-AFCFCD275791}" name="Intraburst Frequency" dataDxfId="0">
+    <tableColumn id="41" xr3:uid="{C175C68A-FBEC-43F7-9A02-AFCFCD275791}" name="Intraburst Frequency" dataDxfId="8">
       <calculatedColumnFormula>1/Table1[[#This Row],[Avg MeanISIinBurst]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="Avg PeakFreqInBurst"/>
@@ -882,6 +1107,27 @@
     <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="Avg BurstsPerSecond"/>
     <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="Include File?"/>
     <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="Include Unit?"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{272AC5AC-EDF2-4DD9-90B7-B026924E4705}" name="Table2" displayName="Table2" ref="A1:F150" totalsRowShown="0" dataDxfId="0" tableBorderDxfId="7">
+  <autoFilter ref="A1:F150" xr:uid="{5FC8953B-5251-4807-A410-510A80EC7D6B}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="CeACRFOA2-5_RD5_12122016_FULL SESSION_Ch0030407_FIN.nex5"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{492973AC-2B13-46B2-B697-17750C6EE42D}" name="Original Filename" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{7159CD58-1C50-44CD-ADC0-23AA0836D1B6}" name="DATA(Q)" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{7C28E939-5898-4FE3-95A3-8BCFCDE13495}" name="units(u)" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00AB6736-D298-4538-B052-60A0D933B4DD}" name="name" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{961FE126-1BDE-411D-BA4A-03C887EAE5A7}" name="drinkType" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{CBDE125F-0C21-4F67-944A-FB0528B7C9B5}" name="drinkDay" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1164,13 +1410,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A9:AO158"/>
   <sheetViews>
-    <sheetView topLeftCell="J4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AK10" sqref="AK10:AK158"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F10" sqref="A10:F158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="88.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
@@ -1332,7 +1578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1461,7 +1707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1589,7 +1835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1717,7 +1963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1845,7 +2091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -1973,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -2229,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -2613,7 +2859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -2869,7 +3115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -2997,7 +3243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -3125,7 +3371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>48</v>
       </c>
@@ -3253,7 +3499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -3509,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -3765,7 +4011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>52</v>
       </c>
@@ -4149,7 +4395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -4405,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -4533,7 +4779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -4661,7 +4907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>53</v>
       </c>
@@ -4789,7 +5035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -5045,7 +5291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -5173,7 +5419,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -5301,7 +5547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>59</v>
       </c>
@@ -5557,7 +5803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>60</v>
       </c>
@@ -5685,7 +5931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -5813,7 +6059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -5941,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -6069,7 +6315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>60</v>
       </c>
@@ -6197,7 +6443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -6325,7 +6571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -6453,7 +6699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>68</v>
       </c>
@@ -6581,7 +6827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>68</v>
       </c>
@@ -6709,7 +6955,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>68</v>
       </c>
@@ -6837,7 +7083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -6965,7 +7211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -7093,7 +7339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -7221,7 +7467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -7349,7 +7595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>68</v>
       </c>
@@ -7477,7 +7723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>68</v>
       </c>
@@ -7605,7 +7851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -7733,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -7861,7 +8107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -8117,7 +8363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>77</v>
       </c>
@@ -8245,7 +8491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>77</v>
       </c>
@@ -8373,7 +8619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -8501,7 +8747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>77</v>
       </c>
@@ -8629,7 +8875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -8757,7 +9003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>77</v>
       </c>
@@ -8885,7 +9131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -9013,7 +9259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -9141,7 +9387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>77</v>
       </c>
@@ -9269,7 +9515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -9525,7 +9771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -9653,7 +9899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>84</v>
       </c>
@@ -9781,7 +10027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>84</v>
       </c>
@@ -9909,7 +10155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>84</v>
       </c>
@@ -10037,7 +10283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>84</v>
       </c>
@@ -10421,7 +10667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>84</v>
       </c>
@@ -10677,7 +10923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -10805,7 +11051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>92</v>
       </c>
@@ -10933,7 +11179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>92</v>
       </c>
@@ -11061,7 +11307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -11317,7 +11563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>92</v>
       </c>
@@ -11573,7 +11819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>94</v>
       </c>
@@ -11701,7 +11947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>94</v>
       </c>
@@ -12213,7 +12459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -12469,7 +12715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -12597,7 +12843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -12725,7 +12971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -12853,7 +13099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -12981,7 +13227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>96</v>
       </c>
@@ -13365,7 +13611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -13621,7 +13867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -14133,7 +14379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -14517,7 +14763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>101</v>
       </c>
@@ -14645,7 +14891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>101</v>
       </c>
@@ -15029,7 +15275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>102</v>
       </c>
@@ -15157,7 +15403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>102</v>
       </c>
@@ -15541,7 +15787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>102</v>
       </c>
@@ -15669,7 +15915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>102</v>
       </c>
@@ -15925,7 +16171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>102</v>
       </c>
@@ -16053,7 +16299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>102</v>
       </c>
@@ -16437,7 +16683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>103</v>
       </c>
@@ -16565,7 +16811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>103</v>
       </c>
@@ -16693,7 +16939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>103</v>
       </c>
@@ -16949,7 +17195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>103</v>
       </c>
@@ -17077,7 +17323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>103</v>
       </c>
@@ -17205,7 +17451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>103</v>
       </c>
@@ -17333,7 +17579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>103</v>
       </c>
@@ -17461,7 +17707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>103</v>
       </c>
@@ -17589,7 +17835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>103</v>
       </c>
@@ -17717,7 +17963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>103</v>
       </c>
@@ -17973,7 +18219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>103</v>
       </c>
@@ -18101,7 +18347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>103</v>
       </c>
@@ -18229,7 +18475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>103</v>
       </c>
@@ -18357,7 +18603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>103</v>
       </c>
@@ -18485,7 +18731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>104</v>
       </c>
@@ -18997,7 +19243,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>104</v>
       </c>
@@ -19637,7 +19883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>104</v>
       </c>
@@ -19765,7 +20011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>107</v>
       </c>
@@ -20021,7 +20267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>107</v>
       </c>
@@ -20149,7 +20395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>107</v>
       </c>
@@ -20277,7 +20523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:41" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>107</v>
       </c>
@@ -20422,60 +20668,3084 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40913BC2-8D3F-4683-A3AC-E9109C96D452}">
+  <dimension ref="A1:F150"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="84.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
+        <v>9</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
+        <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>14</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="6">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
+        <v>18</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="6">
+        <v>3</v>
+      </c>
+      <c r="C10" s="6">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="6">
+        <v>3</v>
+      </c>
+      <c r="C12" s="6">
+        <v>7</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="6">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="6">
+        <v>3</v>
+      </c>
+      <c r="C15" s="6">
+        <v>11</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="6">
+        <v>3</v>
+      </c>
+      <c r="C16" s="6">
+        <v>15</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="6">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6">
+        <v>3</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="6">
+        <v>4</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4</v>
+      </c>
+      <c r="C19" s="6">
+        <v>6</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="6">
+        <v>4</v>
+      </c>
+      <c r="C20" s="6">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" s="6">
+        <v>4</v>
+      </c>
+      <c r="C21" s="6">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="6">
+        <v>4</v>
+      </c>
+      <c r="C22" s="6">
+        <v>12</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="6">
+        <v>6</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="6">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="6">
+        <v>6</v>
+      </c>
+      <c r="C25" s="6">
+        <v>8</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6</v>
+      </c>
+      <c r="C26" s="6">
+        <v>9</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="6">
+        <v>6</v>
+      </c>
+      <c r="C27" s="6">
+        <v>11</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="6">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6">
+        <v>12</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="6">
+        <v>6</v>
+      </c>
+      <c r="C29" s="6">
+        <v>13</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="6">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6">
+        <v>14</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="6">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6">
+        <v>15</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="6">
+        <v>9</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="6">
+        <v>9</v>
+      </c>
+      <c r="C33" s="6">
+        <v>13</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="6">
+        <v>9</v>
+      </c>
+      <c r="C34" s="6">
+        <v>14</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="6">
+        <v>11</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F35" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="6">
+        <v>11</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F36" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="6">
+        <v>11</v>
+      </c>
+      <c r="C37" s="6">
+        <v>3</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F37" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B38" s="6">
+        <v>11</v>
+      </c>
+      <c r="C38" s="6">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F38" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="6">
+        <v>11</v>
+      </c>
+      <c r="C39" s="6">
+        <v>7</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F39" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="6">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6">
+        <v>8</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F40" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B41" s="6">
+        <v>12</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="6">
+        <v>12</v>
+      </c>
+      <c r="C42" s="6">
+        <v>3</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F42" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="6">
+        <v>12</v>
+      </c>
+      <c r="C43" s="6">
+        <v>4</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="6">
+        <v>12</v>
+      </c>
+      <c r="C44" s="6">
+        <v>6</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F44" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="6">
+        <v>12</v>
+      </c>
+      <c r="C45" s="6">
+        <v>8</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F45" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="6">
+        <v>12</v>
+      </c>
+      <c r="C46" s="6">
+        <v>9</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F46" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="6">
+        <v>12</v>
+      </c>
+      <c r="C47" s="6">
+        <v>10</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F47" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="6">
+        <v>12</v>
+      </c>
+      <c r="C48" s="6">
+        <v>13</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F48" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="6">
+        <v>12</v>
+      </c>
+      <c r="C49" s="6">
+        <v>14</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F49" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B50" s="6">
+        <v>12</v>
+      </c>
+      <c r="C50" s="6">
+        <v>15</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F50" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B51" s="6">
+        <v>12</v>
+      </c>
+      <c r="C51" s="6">
+        <v>16</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="6">
+        <v>12</v>
+      </c>
+      <c r="C52" s="6">
+        <v>17</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F52" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="6">
+        <v>13</v>
+      </c>
+      <c r="C53" s="6">
+        <v>1</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F53" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="6">
+        <v>13</v>
+      </c>
+      <c r="C54" s="6">
+        <v>2</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F54" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" s="6">
+        <v>13</v>
+      </c>
+      <c r="C55" s="6">
+        <v>4</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F55" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="6">
+        <v>13</v>
+      </c>
+      <c r="C56" s="6">
+        <v>5</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="6">
+        <v>13</v>
+      </c>
+      <c r="C57" s="6">
+        <v>6</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="6">
+        <v>13</v>
+      </c>
+      <c r="C58" s="6">
+        <v>7</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" s="6">
+        <v>13</v>
+      </c>
+      <c r="C59" s="6">
+        <v>8</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F59" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B60" s="6">
+        <v>13</v>
+      </c>
+      <c r="C60" s="6">
+        <v>9</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F60" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B61" s="6">
+        <v>13</v>
+      </c>
+      <c r="C61" s="6">
+        <v>10</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F61" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B62" s="6">
+        <v>13</v>
+      </c>
+      <c r="C62" s="6">
+        <v>12</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F62" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="6">
+        <v>13</v>
+      </c>
+      <c r="C63" s="6">
+        <v>13</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F63" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B64" s="6">
+        <v>13</v>
+      </c>
+      <c r="C64" s="6">
+        <v>14</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F64" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B65" s="6">
+        <v>14</v>
+      </c>
+      <c r="C65" s="6">
+        <v>3</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F65" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66" s="6">
+        <v>14</v>
+      </c>
+      <c r="C66" s="6">
+        <v>4</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F66" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" s="6">
+        <v>14</v>
+      </c>
+      <c r="C67" s="6">
+        <v>5</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F67" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B68" s="6">
+        <v>14</v>
+      </c>
+      <c r="C68" s="6">
+        <v>6</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B69" s="6">
+        <v>14</v>
+      </c>
+      <c r="C69" s="6">
+        <v>7</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F69" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" s="6">
+        <v>14</v>
+      </c>
+      <c r="C70" s="6">
+        <v>9</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B71" s="6">
+        <v>14</v>
+      </c>
+      <c r="C71" s="6">
+        <v>11</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B72" s="6">
+        <v>14</v>
+      </c>
+      <c r="C72" s="6">
+        <v>14</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F72" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" s="6">
+        <v>14</v>
+      </c>
+      <c r="C73" s="6">
+        <v>15</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F73" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B74" s="6">
+        <v>14</v>
+      </c>
+      <c r="C74" s="6">
+        <v>16</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F74" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B75" s="6">
+        <v>14</v>
+      </c>
+      <c r="C75" s="6">
+        <v>19</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F75" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" s="6">
+        <v>15</v>
+      </c>
+      <c r="C76" s="6">
+        <v>2</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F76" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="6">
+        <v>15</v>
+      </c>
+      <c r="C77" s="6">
+        <v>3</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F77" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78" s="6">
+        <v>15</v>
+      </c>
+      <c r="C78" s="6">
+        <v>5</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F78" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B79" s="6">
+        <v>15</v>
+      </c>
+      <c r="C79" s="6">
+        <v>7</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F79" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B80" s="6">
+        <v>15</v>
+      </c>
+      <c r="C80" s="6">
+        <v>8</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F80" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" s="6">
+        <v>16</v>
+      </c>
+      <c r="C81" s="6">
+        <v>3</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F81" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="6">
+        <v>16</v>
+      </c>
+      <c r="C82" s="6">
+        <v>4</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F82" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="6">
+        <v>16</v>
+      </c>
+      <c r="C83" s="6">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F83" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="6">
+        <v>16</v>
+      </c>
+      <c r="C84" s="6">
+        <v>8</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F84" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="6">
+        <v>16</v>
+      </c>
+      <c r="C85" s="6">
+        <v>10</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F85" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="6">
+        <v>16</v>
+      </c>
+      <c r="C86" s="6">
+        <v>11</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F86" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B87" s="6">
+        <v>17</v>
+      </c>
+      <c r="C87" s="6">
+        <v>1</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F87" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88" s="6">
+        <v>17</v>
+      </c>
+      <c r="C88" s="6">
+        <v>5</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F88" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B89" s="6">
+        <v>17</v>
+      </c>
+      <c r="C89" s="6">
+        <v>6</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F89" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B90" s="6">
+        <v>17</v>
+      </c>
+      <c r="C90" s="6">
+        <v>7</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F90" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B91" s="6">
+        <v>17</v>
+      </c>
+      <c r="C91" s="6">
+        <v>8</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F91" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="6">
+        <v>17</v>
+      </c>
+      <c r="C92" s="6">
+        <v>9</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F92" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="6">
+        <v>17</v>
+      </c>
+      <c r="C93" s="6">
+        <v>11</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F93" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B94" s="6">
+        <v>17</v>
+      </c>
+      <c r="C94" s="6">
+        <v>12</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F94" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B95" s="6">
+        <v>18</v>
+      </c>
+      <c r="C95" s="6">
+        <v>1</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F95" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B96" s="6">
+        <v>19</v>
+      </c>
+      <c r="C96" s="6">
+        <v>1</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E96" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F96" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B97" s="6">
+        <v>19</v>
+      </c>
+      <c r="C97" s="6">
+        <v>2</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E97" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F97" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98" s="6">
+        <v>19</v>
+      </c>
+      <c r="C98" s="6">
+        <v>3</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F98" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B99" s="6">
+        <v>19</v>
+      </c>
+      <c r="C99" s="6">
+        <v>4</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E99" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F99" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100" s="6">
+        <v>19</v>
+      </c>
+      <c r="C100" s="6">
+        <v>5</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F100" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="6">
+        <v>19</v>
+      </c>
+      <c r="C101" s="6">
+        <v>6</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E101" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F101" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6">
+        <v>19</v>
+      </c>
+      <c r="C102" s="6">
+        <v>9</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F102" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" s="6">
+        <v>19</v>
+      </c>
+      <c r="C103" s="6">
+        <v>10</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="E103" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F103" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B104" s="6">
+        <v>19</v>
+      </c>
+      <c r="C104" s="6">
+        <v>11</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F104" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="6">
+        <v>19</v>
+      </c>
+      <c r="C105" s="6">
+        <v>12</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E105" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F105" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B106" s="6">
+        <v>19</v>
+      </c>
+      <c r="C106" s="6">
+        <v>13</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="6">
+        <v>21</v>
+      </c>
+      <c r="C107" s="6">
+        <v>1</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F107" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B108" s="6">
+        <v>21</v>
+      </c>
+      <c r="C108" s="6">
+        <v>2</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F108" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" s="6">
+        <v>21</v>
+      </c>
+      <c r="C109" s="6">
+        <v>3</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E109" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F109" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B110" s="6">
+        <v>21</v>
+      </c>
+      <c r="C110" s="6">
+        <v>4</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F110" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B111" s="6">
+        <v>21</v>
+      </c>
+      <c r="C111" s="6">
+        <v>5</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E111" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F111" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B112" s="6">
+        <v>21</v>
+      </c>
+      <c r="C112" s="6">
+        <v>6</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E112" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F112" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B113" s="6">
+        <v>21</v>
+      </c>
+      <c r="C113" s="6">
+        <v>7</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F113" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B114" s="6">
+        <v>21</v>
+      </c>
+      <c r="C114" s="6">
+        <v>8</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E114" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F114" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B115" s="6">
+        <v>21</v>
+      </c>
+      <c r="C115" s="6">
+        <v>9</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F115" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B116" s="6">
+        <v>21</v>
+      </c>
+      <c r="C116" s="6">
+        <v>11</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F116" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B117" s="6">
+        <v>21</v>
+      </c>
+      <c r="C117" s="6">
+        <v>12</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F117" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B118" s="6">
+        <v>22</v>
+      </c>
+      <c r="C118" s="6">
+        <v>1</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F118" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B119" s="6">
+        <v>22</v>
+      </c>
+      <c r="C119" s="6">
+        <v>2</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F119" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B120" s="6">
+        <v>22</v>
+      </c>
+      <c r="C120" s="6">
+        <v>3</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F120" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" s="6">
+        <v>22</v>
+      </c>
+      <c r="C121" s="6">
+        <v>4</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F121" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" s="6">
+        <v>22</v>
+      </c>
+      <c r="C122" s="6">
+        <v>5</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F122" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B123" s="6">
+        <v>22</v>
+      </c>
+      <c r="C123" s="6">
+        <v>6</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F123" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B124" s="6">
+        <v>22</v>
+      </c>
+      <c r="C124" s="6">
+        <v>7</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F124" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B125" s="6">
+        <v>22</v>
+      </c>
+      <c r="C125" s="6">
+        <v>8</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F125" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B126" s="6">
+        <v>22</v>
+      </c>
+      <c r="C126" s="6">
+        <v>9</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F126" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" s="6">
+        <v>22</v>
+      </c>
+      <c r="C127" s="6">
+        <v>10</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F127" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B128" s="6">
+        <v>22</v>
+      </c>
+      <c r="C128" s="6">
+        <v>11</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F128" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A129" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B129" s="6">
+        <v>22</v>
+      </c>
+      <c r="C129" s="6">
+        <v>12</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F129" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A130" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B130" s="6">
+        <v>22</v>
+      </c>
+      <c r="C130" s="6">
+        <v>13</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F130" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B131" s="6">
+        <v>22</v>
+      </c>
+      <c r="C131" s="6">
+        <v>14</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F131" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B132" s="6">
+        <v>22</v>
+      </c>
+      <c r="C132" s="6">
+        <v>15</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F132" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B133" s="6">
+        <v>22</v>
+      </c>
+      <c r="C133" s="6">
+        <v>16</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F133" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B134" s="6">
+        <v>22</v>
+      </c>
+      <c r="C134" s="6">
+        <v>17</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F134" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B135" s="6">
+        <v>22</v>
+      </c>
+      <c r="C135" s="6">
+        <v>18</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E135" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F135" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B136" s="6">
+        <v>23</v>
+      </c>
+      <c r="C136" s="6">
+        <v>1</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F136" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" s="6">
+        <v>23</v>
+      </c>
+      <c r="C137" s="6">
+        <v>2</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E137" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F137" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B138" s="6">
+        <v>23</v>
+      </c>
+      <c r="C138" s="6">
+        <v>4</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E138" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F138" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A139" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B139" s="6">
+        <v>23</v>
+      </c>
+      <c r="C139" s="6">
+        <v>5</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E139" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F139" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B140" s="6">
+        <v>23</v>
+      </c>
+      <c r="C140" s="6">
+        <v>8</v>
+      </c>
+      <c r="D140" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E140" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F140" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A141" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B141" s="6">
+        <v>23</v>
+      </c>
+      <c r="C141" s="6">
+        <v>12</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F141" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B142" s="6">
+        <v>23</v>
+      </c>
+      <c r="C142" s="6">
+        <v>14</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E142" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F142" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B143" s="6">
+        <v>23</v>
+      </c>
+      <c r="C143" s="6">
+        <v>15</v>
+      </c>
+      <c r="D143" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E143" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F143" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B144" s="6">
+        <v>23</v>
+      </c>
+      <c r="C144" s="6">
+        <v>16</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E144" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F144" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B145" s="6">
+        <v>23</v>
+      </c>
+      <c r="C145" s="6">
+        <v>17</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E145" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F145" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B146" s="6">
+        <v>24</v>
+      </c>
+      <c r="C146" s="6">
+        <v>2</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F146" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B147" s="6">
+        <v>24</v>
+      </c>
+      <c r="C147" s="6">
+        <v>3</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E147" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F147" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A148" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B148" s="6">
+        <v>24</v>
+      </c>
+      <c r="C148" s="6">
+        <v>4</v>
+      </c>
+      <c r="D148" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E148" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F148" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B149" s="6">
+        <v>24</v>
+      </c>
+      <c r="C149" s="6">
+        <v>5</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E149" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F149" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B150" s="6">
+        <v>24</v>
+      </c>
+      <c r="C150" s="6">
+        <v>8</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F150" s="6">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E06D930-766F-4770-9FEC-FB2D7B8BDE57}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>